<commit_message>
added exceljs to project(packages) and completed test for upload/download excell file with assertion
</commit_message>
<xml_diff>
--- a/tests/files/excellDownloadTest.xlsx
+++ b/tests/files/excellDownloadTest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>sno</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Yellow</t>
+  </si>
+  <si>
+    <t>350</t>
   </si>
   <si>
     <t>Summer</t>
@@ -474,11 +477,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>299</v>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,16 +489,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>345</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,16 +506,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>187</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -520,7 +523,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -529,7 +532,7 @@
         <v>350</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -537,16 +540,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>399</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,16 +557,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>